<commit_message>
add results by Google Colab pro plus
</commit_message>
<xml_diff>
--- a/otmm_decimal/result_colab/result_existing_5195_1.0_6_59_ColabFree/a_a_5195_1.0_6_6.xlsx
+++ b/otmm_decimal/result_colab/result_existing_5195_1.0_6_59_ColabFree/a_a_5195_1.0_6_6.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\確率モデル\glycan\otmm_decimal\result_colab\result_existing_5195_1.0_6_59_ColabFree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2151EFE6-F038-4203-AEA4-8769D60D734E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4D0D51-8171-4D48-86A7-825D8D15B7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22560" windowHeight="14440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22560" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="a_a_5195_1.0_6_6" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="179" formatCode="0_);[Red]\(0\)"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -607,11 +620,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -659,7 +675,13 @@
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="良い" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -968,16 +990,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1">
         <v>-6.1000000000000004E-3</v>
       </c>
@@ -997,7 +1022,7 @@
         <v>-40.5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>-99.4</v>
       </c>
@@ -1017,7 +1042,7 @@
         <v>-159</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>-125</v>
       </c>
@@ -1037,7 +1062,7 @@
         <v>-94.8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>-91.3</v>
       </c>
@@ -1057,7 +1082,7 @@
         <v>-0.60799999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>-0.23200000000000001</v>
       </c>
@@ -1077,7 +1102,7 @@
         <v>-1.97</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>-80.2</v>
       </c>
@@ -1095,10 +1120,209 @@
       </c>
       <c r="F6" s="1">
         <v>-11.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3</v>
+      </c>
+      <c r="F8" s="2">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <f>EXP(A1)</f>
+        <v>0.99391856722745398</v>
+      </c>
+      <c r="C9">
+        <f>EXP(B1)</f>
+        <v>6.0967465655156379E-3</v>
+      </c>
+      <c r="D9">
+        <f>EXP(C1)</f>
+        <v>2.5502497662342712E-14</v>
+      </c>
+      <c r="E9">
+        <f>EXP(D1)</f>
+        <v>1.664279891894355E-81</v>
+      </c>
+      <c r="F9">
+        <f>EXP(E1)</f>
+        <v>1.3887943864964021E-11</v>
+      </c>
+      <c r="G9">
+        <f>EXP(F1)</f>
+        <v>2.576757109154981E-18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <f>EXP(A2)</f>
+        <v>6.778420374788599E-44</v>
+      </c>
+      <c r="C10">
+        <f>EXP(B2)</f>
+        <v>4.5517444630832312E-6</v>
+      </c>
+      <c r="D10">
+        <f>EXP(C2)</f>
+        <v>4.3596100000630809E-28</v>
+      </c>
+      <c r="E10">
+        <f>EXP(D2)</f>
+        <v>0.99940117936468509</v>
+      </c>
+      <c r="F10">
+        <f>EXP(E2)</f>
+        <v>5.9318751190738704E-4</v>
+      </c>
+      <c r="G10">
+        <f>EXP(F2)</f>
+        <v>8.8547718835134325E-70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <f>EXP(A3)</f>
+        <v>5.166420632837861E-55</v>
+      </c>
+      <c r="C11">
+        <f>EXP(B3)</f>
+        <v>0.99942116758815391</v>
+      </c>
+      <c r="D11">
+        <f>EXP(C3)</f>
+        <v>8.3152871910356788E-7</v>
+      </c>
+      <c r="E11">
+        <f>EXP(D3)</f>
+        <v>4.4085313314632264E-71</v>
+      </c>
+      <c r="F11">
+        <f>EXP(E3)</f>
+        <v>5.7565617148727611E-4</v>
+      </c>
+      <c r="G11">
+        <f>EXP(F3)</f>
+        <v>6.7434651211919005E-42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="2">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <f>EXP(A4)</f>
+        <v>2.233128952559476E-40</v>
+      </c>
+      <c r="C12">
+        <f>EXP(B4)</f>
+        <v>2.0879679116459336E-14</v>
+      </c>
+      <c r="D12">
+        <f>EXP(C4)</f>
+        <v>1.5647957103941666E-3</v>
+      </c>
+      <c r="E12">
+        <f>EXP(D4)</f>
+        <v>0.45384479528235583</v>
+      </c>
+      <c r="F12">
+        <f>EXP(E4)</f>
+        <v>3.0590232050182579E-7</v>
+      </c>
+      <c r="G12">
+        <f>EXP(F4)</f>
+        <v>0.54443865823921711</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="2">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <f>EXP(A5)</f>
+        <v>0.79294612330668368</v>
+      </c>
+      <c r="C13">
+        <f>EXP(B5)</f>
+        <v>7.6218651945128903E-12</v>
+      </c>
+      <c r="D13">
+        <f>EXP(C5)</f>
+        <v>1.1881323302462067E-28</v>
+      </c>
+      <c r="E13">
+        <f>EXP(D5)</f>
+        <v>2.4069765506104637E-69</v>
+      </c>
+      <c r="F13">
+        <f>EXP(E5)</f>
+        <v>6.6536806715016855E-2</v>
+      </c>
+      <c r="G13">
+        <f>EXP(F5)</f>
+        <v>0.13945685621505094</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="2">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <f>EXP(A6)</f>
+        <v>1.4776873359645133E-35</v>
+      </c>
+      <c r="C14">
+        <f>EXP(B6)</f>
+        <v>1.713908431542013E-15</v>
+      </c>
+      <c r="D14">
+        <f>EXP(C6)</f>
+        <v>6.9322975975865472E-14</v>
+      </c>
+      <c r="E14">
+        <f>EXP(D6)</f>
+        <v>4.2483542552915889E-18</v>
+      </c>
+      <c r="F14">
+        <f>EXP(E6)</f>
+        <v>0.9999915700355323</v>
+      </c>
+      <c r="G14">
+        <f>EXP(F6)</f>
+        <v>8.2938191607573704E-6</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>
+  <conditionalFormatting sqref="B9:G14">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
+      <formula>0.3</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>